<commit_message>
fix code and pptx
</commit_message>
<xml_diff>
--- a/Homework 1/dataframe/Exams.xlsx
+++ b/Homework 1/dataframe/Exams.xlsx
@@ -5,23 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\Università\Visual Analytics\HW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\Università\Visual Analytics\VisualAnalytics_HW\Homework 1\dataframe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FC4847-8E3F-4E7E-BECA-85D4EE387C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB849275-6961-4F9B-910D-51FC35E4AEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2052" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ernest" sheetId="3" r:id="rId1"/>
     <sheet name="Francesco" sheetId="1" r:id="rId2"/>
     <sheet name="Giacomo" sheetId="4" r:id="rId3"/>
+    <sheet name="Group" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="DatiEsterni_1" localSheetId="0" hidden="1">Ernest!$A$1:$F$18</definedName>
     <definedName name="DatiEsterni_1" localSheetId="2" hidden="1">Giacomo!$A$1:$F$18</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>Exam Number</t>
   </si>
@@ -109,6 +121,57 @@
   </si>
   <si>
     <t>Credits</t>
+  </si>
+  <si>
+    <t>18/02/2019</t>
+  </si>
+  <si>
+    <t>12/06/2019</t>
+  </si>
+  <si>
+    <t>11/02/2020</t>
+  </si>
+  <si>
+    <t>12/02/2020</t>
+  </si>
+  <si>
+    <t>12/06/2020</t>
+  </si>
+  <si>
+    <t>22/06/2020</t>
+  </si>
+  <si>
+    <t>15/07/2020</t>
+  </si>
+  <si>
+    <t>13/01/2021</t>
+  </si>
+  <si>
+    <t>17/01/2021</t>
+  </si>
+  <si>
+    <t>25/01/2021</t>
+  </si>
+  <si>
+    <t>14/06/2021</t>
+  </si>
+  <si>
+    <t>09/07/2021</t>
+  </si>
+  <si>
+    <t>21/07/2021</t>
+  </si>
+  <si>
+    <t>18/01/2022</t>
+  </si>
+  <si>
+    <t>26/01/2022</t>
+  </si>
+  <si>
+    <t>06/06/2022</t>
+  </si>
+  <si>
+    <t>21/06/2022</t>
   </si>
 </sst>
 </file>
@@ -162,12 +225,30 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -182,9 +263,6 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -192,9 +270,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1259,12 +1334,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{991C4492-4997-4D0A-B758-F7CBE771FE08}" name="New" displayName="New" ref="A1:F18" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F18" xr:uid="{991C4492-4997-4D0A-B758-F7CBE771FE08}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D7B6CDE8-31FD-4B69-A25F-1CD504EE9913}" uniqueName="1" name="Exam Number" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{74F52EF8-6DBC-47B4-B58B-BA2053F91420}" uniqueName="2" name="Exam Code" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{0ACAFE1C-7B6A-4485-9B50-42325F80427E}" uniqueName="3" name="Name" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{F2C9BADD-EF76-4AA5-B0E3-84FC4326D06B}" uniqueName="4" name="Date" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{D7B6CDE8-31FD-4B69-A25F-1CD504EE9913}" uniqueName="1" name="Exam Number" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{74F52EF8-6DBC-47B4-B58B-BA2053F91420}" uniqueName="2" name="Exam Code" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{0ACAFE1C-7B6A-4485-9B50-42325F80427E}" uniqueName="3" name="Name" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{F2C9BADD-EF76-4AA5-B0E3-84FC4326D06B}" uniqueName="4" name="Date" queryTableFieldId="4" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{FC818720-43A9-4315-95CB-E264C081D5D4}" uniqueName="5" name="Grade" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{76D241A9-B71A-4B83-802E-A4B8A8F14FC5}" uniqueName="6" name="Credits" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{76D241A9-B71A-4B83-802E-A4B8A8F14FC5}" uniqueName="6" name="Credits" queryTableFieldId="6" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1274,12 +1349,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E9078B69-6994-4D1F-9EEF-9A890E7A6DB0}" name="Tabella2" displayName="Tabella2" ref="A1:F18" totalsRowShown="0">
   <autoFilter ref="A1:F18" xr:uid="{E9078B69-6994-4D1F-9EEF-9A890E7A6DB0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D825CE0F-8BB5-4E25-AB23-2A69F7EA0BE1}" name="Exam Number" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{571C6FB7-613A-4C77-AA8C-1F3848303F43}" name="Exam Code" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{D825CE0F-8BB5-4E25-AB23-2A69F7EA0BE1}" name="Exam Number" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{571C6FB7-613A-4C77-AA8C-1F3848303F43}" name="Exam Code" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{45A842D6-D020-4993-99BC-9311FB7E99A5}" name="Name"/>
-    <tableColumn id="4" xr3:uid="{DCD94814-664C-41BE-A5C2-785B0D426617}" name="Date" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DCD94814-664C-41BE-A5C2-785B0D426617}" name="Date" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{6DB750DC-03AB-4E7F-99D9-0C572B0087A9}" name="Grade"/>
-    <tableColumn id="6" xr3:uid="{530710CE-677B-4C13-A250-08116288CB71}" name="Credits" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{530710CE-677B-4C13-A250-08116288CB71}" name="Credits" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1289,12 +1364,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AFEA62E8-2A17-4697-A61D-7C57737048E1}" name="New__2" displayName="New__2" ref="A1:F18" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F18" xr:uid="{AFEA62E8-2A17-4697-A61D-7C57737048E1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E010DB77-D7B7-4984-86AD-35A41AF197C5}" uniqueName="1" name="Exam Number" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{B251E487-B4CD-4AA9-8038-344FE8B85422}" uniqueName="2" name="Exam Code" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4086EC34-372F-44A0-9840-41710A496CE9}" uniqueName="3" name="Name" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{8F978278-E1C8-41BB-A63D-4232CAB1933B}" uniqueName="4" name="Date" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E010DB77-D7B7-4984-86AD-35A41AF197C5}" uniqueName="1" name="Exam Number" queryTableFieldId="1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B251E487-B4CD-4AA9-8038-344FE8B85422}" uniqueName="2" name="Exam Code" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4086EC34-372F-44A0-9840-41710A496CE9}" uniqueName="3" name="Name" queryTableFieldId="3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{8F978278-E1C8-41BB-A63D-4232CAB1933B}" uniqueName="4" name="Date" queryTableFieldId="4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{7D9B5CB9-4E5A-4E23-BB7C-F38C07B6D3A0}" uniqueName="5" name="Grade" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{35353973-3A29-4A35-9768-83475C3D6170}" uniqueName="6" name="Credits" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{35353973-3A29-4A35-9768-83475C3D6170}" uniqueName="6" name="Credits" queryTableFieldId="6" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F08E6FD2-66DD-402A-9197-8CEDA7F48DDD}" name="Tabella25" displayName="Tabella25" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{F08E6FD2-66DD-402A-9197-8CEDA7F48DDD}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{9238877F-04A0-43A7-AAE1-1BD2CABE05A3}" name="Exam Number" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A77CB3AE-DB11-42D8-BF20-4198ECD17CDA}" name="Exam Code" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{AC12F7CF-9C31-422C-9170-1DFC349533AB}" name="Name"/>
+    <tableColumn id="4" xr3:uid="{7852D917-27CB-4153-88D1-6074923EBAAD}" name="Date" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FE9683CB-0802-46D7-8E83-A8D48F34D0FD}" name="Grade">
+      <calculatedColumnFormula>AVERAGE(Ernest!E2,Francesco!E2,Giacomo!E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{ECD9C247-B6BB-4E4B-B1F8-FF9FD0D9C52F}" name="Credits" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1624,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECD8A96-979E-46E5-B74F-251DED46E139}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2012,7 +2104,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2461,7 +2553,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2828,6 +2920,408 @@
       </c>
       <c r="E18">
         <v>23</v>
+      </c>
+      <c r="F18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FE852D-E885-45F6-85B8-2D1C3DCCF9DC}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" customWidth="1"/>
+    <col min="3" max="3" width="38.796875" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>101204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(Ernest!E2,Francesco!E2,Giacomo!E2)</f>
+        <v>20.666666666666668</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1056025</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(Ernest!E3,Francesco!E3,Giacomo!E3)</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1017218</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <f>AVERAGE(Ernest!E4,Francesco!E4,Giacomo!E4)</f>
+        <v>24.333333333333332</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1018706</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <f>AVERAGE(Ernest!E5,Francesco!E5,Giacomo!E5)</f>
+        <v>21.666666666666668</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1056029</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(Ernest!E6,Francesco!E6,Giacomo!E6)</f>
+        <v>22</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1017219</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <f>AVERAGE(Ernest!E7,Francesco!E7,Giacomo!E7)</f>
+        <v>26</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1017400</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(Ernest!E8,Francesco!E8,Giacomo!E8)</f>
+        <v>23.666666666666668</v>
+      </c>
+      <c r="F8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1017398</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <f>AVERAGE(Ernest!E9,Francesco!E9,Giacomo!E9)</f>
+        <v>20.333333333333332</v>
+      </c>
+      <c r="F9" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1041469</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(Ernest!E10,Francesco!E10,Giacomo!E10)</f>
+        <v>25.666666666666668</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1015392</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <f>AVERAGE(Ernest!E11,Francesco!E11,Giacomo!E11)</f>
+        <v>29</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1021946</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(Ernest!E12,Francesco!E12,Giacomo!E12)</f>
+        <v>26.333333333333332</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1018745</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(Ernest!E13,Francesco!E13,Giacomo!E13)</f>
+        <v>26</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1018733</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <f>AVERAGE(Ernest!E14,Francesco!E14,Giacomo!E14)</f>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1022563</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(Ernest!E15,Francesco!E15,Giacomo!E15)</f>
+        <v>22.333333333333332</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1056030</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(Ernest!E16,Francesco!E16,Giacomo!E16)</f>
+        <v>25</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1016596</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(Ernest!E17,Francesco!E17,Giacomo!E17)</f>
+        <v>27.666666666666668</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1056028</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <f>AVERAGE(Ernest!E18,Francesco!E18,Giacomo!E18)</f>
+        <v>24.666666666666668</v>
       </c>
       <c r="F18" s="1">
         <v>9</v>

</xml_diff>